<commit_message>
added multi formation energy
</commit_message>
<xml_diff>
--- a/plotpackage/data/formation_energy.xlsx
+++ b/plotpackage/data/formation_energy.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Formation Energy" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>single doping in the first layer</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>Pt</t>
+  </si>
+  <si>
+    <t>single doping in the subsurface</t>
+  </si>
+  <si>
+    <t>overlayer</t>
+  </si>
+  <si>
+    <t>island</t>
+  </si>
+  <si>
+    <t>subsurface</t>
+  </si>
+  <si>
+    <t>parallelogram</t>
+  </si>
+  <si>
+    <t>Ti</t>
+  </si>
+  <si>
+    <t>Hf</t>
   </si>
 </sst>
 </file>
@@ -365,73 +386,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>5.5496137499985387E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>0.1092539975000042</v>
+      </c>
+      <c r="D2">
+        <v>0.36753135638888895</v>
+      </c>
+      <c r="E2">
+        <v>0.22382353250000531</v>
+      </c>
+      <c r="F2">
+        <v>0.31063214194444516</v>
+      </c>
+      <c r="G2">
+        <v>0.2323341250000075</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>0.48683692500000753</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>0.56391413500003473</v>
+      </c>
+      <c r="D3">
+        <v>0.72377658944444911</v>
+      </c>
+      <c r="E3">
+        <v>0.64230312499999975</v>
+      </c>
+      <c r="F3">
+        <v>0.65973504166667263</v>
+      </c>
+      <c r="G3">
+        <v>0.60245007000000506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>-0.13188766499997673</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>-0.20281884499997904</v>
+      </c>
+      <c r="D4">
+        <v>-0.2061410638888839</v>
+      </c>
+      <c r="E4">
+        <v>-6.6620834999992162E-2</v>
+      </c>
+      <c r="F4">
+        <v>-0.27891608944444474</v>
+      </c>
+      <c r="G4">
+        <v>-4.0901902499993703E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>-5.829132499996259E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>-0.13964059499999504</v>
+      </c>
+      <c r="D5">
+        <v>0.3022197727777779</v>
+      </c>
+      <c r="E5">
+        <v>0.1503021475000077</v>
+      </c>
+      <c r="F5">
+        <v>0.39943862388889273</v>
+      </c>
+      <c r="G5">
+        <v>0.20930033750000465</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>-0.45645074637928573</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>-0.71314150637931206</v>
+      </c>
+      <c r="D6">
+        <v>-9.2570241570888202E-3</v>
+      </c>
+      <c r="E6">
+        <v>-0.14955614637930736</v>
+      </c>
+      <c r="F6">
+        <v>5.4509480287357408E-2</v>
+      </c>
+      <c r="G6">
+        <v>-9.9625411379303586E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0.39462549499999344</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>0.37280091500000712</v>
+      </c>
+      <c r="D7">
+        <v>0.47790880055555796</v>
+      </c>
+      <c r="E7">
+        <v>0.53287292750000237</v>
+      </c>
+      <c r="F7">
+        <v>0.42017660611111096</v>
+      </c>
+      <c r="G7">
+        <v>0.49975075000001201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>-0.15383427249997261</v>
+      </c>
+      <c r="C8">
+        <v>0.22755464750003362</v>
+      </c>
+      <c r="D8">
+        <v>0.2846047808333374</v>
+      </c>
+      <c r="E8">
+        <v>8.2740877500006249E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.52999399083333487</v>
+      </c>
+      <c r="G8">
+        <v>0.12850357000001189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>-1.0553793694444416</v>
+      </c>
+      <c r="E9">
+        <v>-1.1420011749999892</v>
+      </c>
+      <c r="F9">
+        <v>-1.0078864494444422</v>
+      </c>
+      <c r="G9">
+        <v>-1.0807497274999909</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-0.76025394722222039</v>
+      </c>
+      <c r="E10">
+        <v>-1.5250302849999908</v>
+      </c>
+      <c r="F10">
+        <v>-0.65028787499999929</v>
+      </c>
+      <c r="G10">
+        <v>-1.4776542124999903</v>
       </c>
     </row>
   </sheetData>

</xml_diff>